<commit_message>
Tela saber mais e outras melhorias
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/basededados.xlsx
+++ b/app/src/main/res/raw/basededados.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t xml:space="preserve">node_id</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">DELGADO</t>
   </si>
   <si>
-    <t xml:space="preserve">Esse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahuEsse é um texto que supostamente ajuda. 1 asudhahuds shuuhsahu sdhushudhusa husduhsuhsd hushusuh husdhusdhuas uhasdhusdhu huasdhusahus husadhusdahusd sdahusdahusahu</t>
+    <t xml:space="preserve">Esse é um texto que supostamente ajuda. 1</t>
   </si>
   <si>
     <t xml:space="preserve">O Corg provém de acumulações naturais de resíduos vegetais?</t>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t xml:space="preserve">A seção rica em Corg está à superfície do solo?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FINAL </t>
   </si>
   <si>
     <t xml:space="preserve">Esse é um texto que supostamente ajuda. 5</t>
@@ -150,7 +147,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;BOOL&quot;e&quot;AN&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -187,12 +184,6 @@
       <name val="Inconsolata"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Inconsolata"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -243,7 +234,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -265,10 +256,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,10 +281,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="86.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.52"/>
@@ -353,7 +340,7 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="3"/>
@@ -418,7 +405,7 @@
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -484,13 +471,13 @@
         <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4"/>
@@ -514,17 +501,17 @@
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>24</v>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
@@ -549,16 +536,16 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
@@ -580,19 +567,19 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>32</v>
+      <c r="D9" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4"/>
@@ -613,20 +600,20 @@
       <c r="V9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
-        <v>32</v>
+      <c r="A10" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4"/>
@@ -648,19 +635,19 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="4"/>
@@ -682,19 +669,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>

</xml_diff>